<commit_message>
Check in part 4
</commit_message>
<xml_diff>
--- a/Topics.xlsx
+++ b/Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhilajoseph/Documents/DS/Projects/Akhila-Joseph-Projects/Project_5/Covid-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41BC9046-D748-9246-8BDB-0F89D68624EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1BF756-6794-0944-9AB4-23CCE4457041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{297854A1-58F4-AB43-AAA3-F14ABD3A8DF4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
   <si>
     <t>Spread in US</t>
   </si>
@@ -300,6 +300,18 @@
   </si>
   <si>
     <t>Cases</t>
+  </si>
+  <si>
+    <t>Areas of improvements?</t>
+  </si>
+  <si>
+    <t>Does prediction makes sense in an exponential model - LSTM</t>
+  </si>
+  <si>
+    <t>what else would you like to see for yourself in a similar study?</t>
+  </si>
+  <si>
+    <t>Any other insights on getting more data sources?</t>
   </si>
 </sst>
 </file>
@@ -660,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E867B4F1-CA35-E04E-A997-68BEB4995D6E}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,6 +685,7 @@
     <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -936,7 +949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>64</v>
       </c>
@@ -950,7 +963,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>30</v>
       </c>
@@ -964,7 +977,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>32</v>
       </c>
@@ -978,7 +991,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>65</v>
       </c>
@@ -992,7 +1005,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>66</v>
       </c>
@@ -1003,7 +1016,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>74</v>
       </c>
@@ -1011,7 +1024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>75</v>
       </c>
@@ -1019,9 +1032,29 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>